<commit_message>
Improved Fitness and Selector with more mutations
</commit_message>
<xml_diff>
--- a/Time_Table.xlsx
+++ b/Time_Table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Class</t>
   </si>
@@ -32,112 +32,106 @@
     <t>Time</t>
   </si>
   <si>
+    <t>Azmayieshgah_riyazi</t>
+  </si>
+  <si>
+    <t>Wendsday</t>
+  </si>
+  <si>
+    <t>Teacher8</t>
+  </si>
+  <si>
+    <t>14 - 16</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>Teacher7</t>
+  </si>
+  <si>
+    <t>16 - 18</t>
+  </si>
+  <si>
+    <t>Compiler</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Teacher9</t>
+  </si>
+  <si>
+    <t>Tarkibiyat</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Madar_Manteghi</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Teacher1</t>
+  </si>
+  <si>
+    <t>Data_Structure</t>
+  </si>
+  <si>
+    <t>Teacher6</t>
+  </si>
+  <si>
+    <t>10 - 12</t>
+  </si>
+  <si>
+    <t>Riyazi3</t>
+  </si>
+  <si>
+    <t>Phisics</t>
+  </si>
+  <si>
+    <t>Teacher2</t>
+  </si>
+  <si>
+    <t>8 - 10</t>
+  </si>
+  <si>
+    <t>Mabani_Nazariye_Mohasebe</t>
+  </si>
+  <si>
+    <t>Satureday</t>
+  </si>
+  <si>
+    <t>Mabani_Matrix</t>
+  </si>
+  <si>
+    <t>Numerical Analyises</t>
+  </si>
+  <si>
+    <t>Riyazi2</t>
+  </si>
+  <si>
+    <t>Teacher3</t>
+  </si>
+  <si>
+    <t>Pishrafte</t>
+  </si>
+  <si>
     <t>Kargahe_Computer</t>
   </si>
   <si>
-    <t>Wendsday</t>
-  </si>
-  <si>
-    <t>Teacher7</t>
-  </si>
-  <si>
-    <t>8 - 10</t>
+    <t>Riyzi1</t>
+  </si>
+  <si>
+    <t>mabani_computer</t>
   </si>
   <si>
     <t>Mabani_Riazi</t>
   </si>
   <si>
-    <t>Teacher1</t>
-  </si>
-  <si>
-    <t>14 - 16</t>
-  </si>
-  <si>
-    <t>Mabani_Matrix</t>
-  </si>
-  <si>
-    <t>Teacher4</t>
-  </si>
-  <si>
-    <t>16 - 18</t>
-  </si>
-  <si>
-    <t>Tarkibiyat</t>
-  </si>
-  <si>
-    <t>Satureday</t>
-  </si>
-  <si>
-    <t>Teacher8</t>
-  </si>
-  <si>
-    <t>10 - 12</t>
-  </si>
-  <si>
     <t>moadelat</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Phisics</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Teacher2</t>
-  </si>
-  <si>
-    <t>Madar_Manteghi</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Riyazi2</t>
-  </si>
-  <si>
-    <t>Azmayieshgah_riyazi</t>
-  </si>
-  <si>
-    <t>Teacher6</t>
-  </si>
-  <si>
-    <t>Mabani_Nazariye_Mohasebe</t>
-  </si>
-  <si>
-    <t>Numerical Analyises</t>
-  </si>
-  <si>
-    <t>Teacher3</t>
-  </si>
-  <si>
-    <t>Data_Structure</t>
-  </si>
-  <si>
-    <t>mabani_computer</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>Riyazi3</t>
-  </si>
-  <si>
-    <t>Teacher9</t>
-  </si>
-  <si>
-    <t>Pishrafte</t>
-  </si>
-  <si>
-    <t>Teacher5</t>
-  </si>
-  <si>
-    <t>Riyzi1</t>
-  </si>
-  <si>
-    <t>Compiler</t>
   </si>
 </sst>
 </file>
@@ -486,7 +480,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,13 +547,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -573,10 +567,10 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -584,98 +578,98 @@
         <v>100</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -683,67 +677,67 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -751,101 +745,101 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
         <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="n">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -853,257 +847,53 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
         <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="n">
-        <v>110</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="n">
-        <v>110</v>
-      </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="n">
-        <v>115</v>
-      </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="n">
-        <v>115</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="n">
-        <v>115</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="n">
-        <v>115</v>
-      </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="n">
-        <v>115</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="n">
-        <v>115</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="n">
-        <v>115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="n">
-        <v>115</v>
-      </c>
-      <c r="B34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="n">
-        <v>115</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="n">
-        <v>120</v>
-      </c>
-      <c r="B36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>